<commit_message>
Made small changes in index.html
</commit_message>
<xml_diff>
--- a/WorkOrganization/WorkflowAndResponsibilities.xlsx
+++ b/WorkOrganization/WorkflowAndResponsibilities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veso\Drive\(0)TelerikAcademy\(11) JS Apps\JS-Apps-Teamwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veso\Drive\(0)TelerikAcademy\(11) JS Apps\JS-Apps-Teamwork\WorkOrganization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Track (Geri)</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>30.08.2015</t>
+  </si>
+  <si>
+    <t>log in page</t>
   </si>
 </sst>
 </file>
@@ -409,6 +412,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -420,21 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,7 +997,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,50 +1018,50 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="63" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1069,28 +1072,28 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="9"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -1098,26 +1101,26 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="9"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1125,24 +1128,24 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="9"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1150,20 +1153,22 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="11"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="9"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1177,23 +1182,23 @@
       <c r="B8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="12"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="8" t="s">
         <v>23</v>
       </c>

</xml_diff>